<commit_message>
SN: Update Sénégal TAS1 form
</commit_message>
<xml_diff>
--- a/LF/TAS/Senegal/TAS2/Avr 2021/sn_lf_tas1_2_partcipants_202104.xlsx
+++ b/LF/TAS/Senegal/TAS2/Avr 2021/sn_lf_tas1_2_partcipants_202104.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Senegal\TAS2\Avr 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0506D43-4FAA-435F-ADB4-10A471A8268A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6D776F-9CB8-4755-A3E2-4CEBA64A275A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
   <si>
     <t>form_title</t>
   </si>
@@ -344,13 +344,22 @@
     <t>L'age doit être compris entre 5 et 9 ans</t>
   </si>
   <si>
-    <t>sn_lf_tas1_2_partcipants_202104</t>
-  </si>
-  <si>
-    <t>(Avril 2021) 2. TAS1 FL - Formulaire Participants</t>
-  </si>
-  <si>
     <t>concat(${p_cluster_id},'-',substr(random(),3,10))</t>
+  </si>
+  <si>
+    <t>p_commune</t>
+  </si>
+  <si>
+    <t>Select your commune</t>
+  </si>
+  <si>
+    <t>Sélectionner votre commune</t>
+  </si>
+  <si>
+    <t>sn_lf_tas1_2_partcipants_202104_v2</t>
+  </si>
+  <si>
+    <t>(Avril 2021) 2. TAS1 FL - Formulaire Participants V2</t>
   </si>
 </sst>
 </file>
@@ -862,13 +871,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1012,14 +1021,14 @@
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="12"/>
@@ -1036,81 +1045,79 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C6" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="31" t="s">
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-    </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
     </row>
     <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="9" t="s">
         <v>80</v>
@@ -1119,121 +1126,121 @@
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>103</v>
-      </c>
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-    </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>43</v>
+      <c r="B9" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="16" t="s">
-        <v>77</v>
+        <v>42</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>48</v>
+        <v>67</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="8"/>
@@ -1241,7 +1248,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
@@ -1251,104 +1258,112 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>106</v>
-      </c>
+      <c r="K12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="8"/>
       <c r="M12" s="9" t="s">
         <v>80</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
-      <c r="P12" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
+      <c r="K13" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="K14" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="M14" s="9"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="20"/>
+        <v>52</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="21" t="s">
+        <v>58</v>
+      </c>
       <c r="F15" s="21"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1361,27 +1376,49 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1518,7 +1555,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1544,10 +1581,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C2">
         <v>20210419</v>

</xml_diff>